<commit_message>
added summary rpt pkg and updated total row to total by property instead of unit type
</commit_message>
<xml_diff>
--- a/rx_PSC_RentalActivity_Sum.xlsx
+++ b/rx_PSC_RentalActivity_Sum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-RentalActivity-YSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D0DBBC-B83D-4138-B4B3-3E6C897C5E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46F4AFA-2CAE-4B1E-826F-D31C8DBE8031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2730" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PS" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
-  <si>
-    <t>Rental Activity</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Unit Type</t>
   </si>
@@ -161,46 +158,52 @@
     <t>&amp;=display.Property_Code</t>
   </si>
   <si>
-    <t>&amp;=&amp;=SUMIF(C5:C{-1}, 1, D5:D{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(C5:C{-1}, 1, E5:E{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(C5:C{-1}, 1, F5:F{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(C5:C{-1}, 1, G5:G{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(C5:C{-1}, 1, H5:H{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(C5:C{-1}, 1, I5:I{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(C5:C{-1}, 1, J5:J{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(C5:C{-1}, 1, K5:K{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(C5:C{-1}, 1, L5:L{-1})/SUM(C5:C{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(C5:C{-1},1, M5:M{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(C5:C{-1}, 1, N5:N{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(C5:C{-1}, 1, O5:O{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(C5:C{-1}, 1, P5:P{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(C5:C{-1}, 1, Q5:Q{-1})</t>
+    <t>Count of Distinct Properties</t>
+  </si>
+  <si>
+    <t>Rental Activity Summary</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, E5:E{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, F5:F{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, G5:G{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, H5:H{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, I5:I{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, J5:J{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, K5:K{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, L5:L{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, M5:M{-1})/SUM(B5:B{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1},1, N5:N{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, O5:O{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, P5:P{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, Q5:Q{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, R5:R{-1})</t>
   </si>
 </sst>
 </file>
@@ -647,35 +650,35 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="3" max="3" width="88.08984375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" customWidth="1"/>
-    <col min="10" max="10" width="7.54296875" customWidth="1"/>
-    <col min="11" max="12" width="7.81640625" customWidth="1"/>
-    <col min="13" max="13" width="12.7265625" customWidth="1"/>
-    <col min="14" max="14" width="7.54296875" customWidth="1"/>
-    <col min="15" max="15" width="9.453125" customWidth="1"/>
-    <col min="16" max="16" width="12.7265625" customWidth="1"/>
-    <col min="17" max="17" width="9.26953125" customWidth="1"/>
-    <col min="18" max="18" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="37.90625" customWidth="1"/>
+    <col min="6" max="6" width="9.08984375" customWidth="1"/>
+    <col min="7" max="7" width="7.453125" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" customWidth="1"/>
+    <col min="9" max="9" width="8.453125" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" customWidth="1"/>
+    <col min="11" max="11" width="7.54296875" customWidth="1"/>
+    <col min="12" max="13" width="7.81640625" customWidth="1"/>
+    <col min="14" max="14" width="12.7265625" customWidth="1"/>
+    <col min="15" max="15" width="7.54296875" customWidth="1"/>
+    <col min="16" max="16" width="9.453125" customWidth="1"/>
+    <col min="17" max="17" width="12.7265625" customWidth="1"/>
+    <col min="18" max="18" width="9.26953125" customWidth="1"/>
+    <col min="19" max="19" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -694,10 +697,11 @@
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
     </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -716,10 +720,11 @@
       <c r="P2" s="13"/>
       <c r="Q2" s="13"/>
       <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
     </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -738,128 +743,132 @@
       <c r="P3" s="13"/>
       <c r="Q3" s="13"/>
       <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="B5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="H5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>25</v>
+      <c r="Q5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="3" t="s">
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="6" t="s">
         <v>42</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -880,36 +889,39 @@
       <c r="K6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="9" t="s">
         <v>50</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="O6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="P6" s="10" t="s">
         <v>53</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="R6" s="3"/>
+      <c r="R6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="S6" s="3"/>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" t="s">
-        <v>28</v>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A3:R3"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:S2"/>
+    <mergeCell ref="A3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.7" bottom="0.7" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="990" orientation="portrait" useFirstPageNumber="1"/>
@@ -921,7 +933,7 @@
     <brk id="29" max="16383" man="1"/>
   </rowBreaks>
   <ignoredErrors>
-    <ignoredError sqref="D4:E4 B4 P4:Q4 H4:K4" numberStoredAsText="1"/>
+    <ignoredError sqref="E4:F4 C4 Q4:R4 I4:L4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>